<commit_message>
Updated BLP Forecasting download functionality
git-svn-id: http://mslinuxdb01.macrosynergy.local/repositories/Nowcast/trunk@200 b65b143d-dad5-48b2-bbf2-81d1f728c7de
</commit_message>
<xml_diff>
--- a/data/Bloomberg Forecasts.xlsx
+++ b/data/Bloomberg Forecasts.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="37395" windowHeight="20490"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <pivotCaches>
+    <pivotCache cacheId="3" r:id="rId5"/>
+  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="151">
   <si>
     <t>US Forecasts</t>
   </si>
@@ -466,6 +470,9 @@
   </si>
   <si>
     <t>Ticker</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
   </si>
 </sst>
 </file>
@@ -509,9 +516,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,6 +560,1032 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Lasse de la Porte Simonsen" refreshedDate="42901.516677314816" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="74">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:C75" sheet="Sheet1"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="US Forecasts" numFmtId="0">
+      <sharedItems count="74">
+        <s v="Banco Bradesco"/>
+        <s v="Action Economics"/>
+        <s v="Avalon Advisors"/>
+        <s v="AXA Investment Managers"/>
+        <s v="Bank of America Merrillynch"/>
+        <s v="Bank of the West"/>
+        <s v="Barclays"/>
+        <s v="BBVA Research"/>
+        <s v="Berenberg Bank"/>
+        <s v="Bloomberg Intelligence"/>
+        <s v="BMO Capital"/>
+        <s v="Canadian Imperial Bank"/>
+        <s v="Capital Economics"/>
+        <s v="CME Group"/>
+        <s v="Comerica"/>
+        <s v="Conference Board"/>
+        <s v="Credit Agricole CIB"/>
+        <s v="Credit Suisse Group"/>
+        <s v="Desjardins Securities"/>
+        <s v="Deutche Bank"/>
+        <s v="Euler Hermes"/>
+        <s v="Fannie Mae"/>
+        <s v="First Trust Advisors"/>
+        <s v="FTN Financial"/>
+        <s v="Georgia State University"/>
+        <s v="Goldman Sachs Group"/>
+        <s v="Helaba Bank"/>
+        <s v="High Frequency Economics"/>
+        <s v="Hugh Johnson Advisors"/>
+        <s v="HIS Economics"/>
+        <s v="ING Group"/>
+        <s v="JPMorgan Chase"/>
+        <s v="Kennesaw State University"/>
+        <s v="KPMG"/>
+        <s v="Macroeconomic Advisers"/>
+        <s v="MacroFin Analytics LLC"/>
+        <s v="Moody's"/>
+        <s v="MUFG"/>
+        <s v="Naroff Economic Advisors"/>
+        <s v="National Association of Home Builders"/>
+        <s v="National Bank Financial"/>
+        <s v="Natl Truck Equipment"/>
+        <s v="Nomura Securities"/>
+        <s v="Norddeutsche Landesbank"/>
+        <s v="Oxford Economics"/>
+        <s v="Pantheon Macroeconomics"/>
+        <s v="Parsec Financial Management"/>
+        <s v="Pierpont Securities"/>
+        <s v="Piper Jaffray &amp; Co."/>
+        <s v="Prestige Economics LLC"/>
+        <s v="Rabobank"/>
+        <s v="Raiffeisen Zentralbank"/>
+        <s v="Raymond James Financial"/>
+        <s v="RBC Financial Group"/>
+        <s v="Regions Financial"/>
+        <s v="Scotia Capital"/>
+        <s v="SMBC Nikko"/>
+        <s v="Stifel Financial"/>
+        <s v="Swiss Reinsurance"/>
+        <s v="TD Securities"/>
+        <s v="UMB Bank"/>
+        <s v="UniCredit"/>
+        <s v="University of Maryland"/>
+        <s v="University of Texas/El P"/>
+        <s v="US Chamber of Commerce"/>
+        <s v="Vinning Sparks"/>
+        <s v="Wells Fargo"/>
+        <s v="Citigroup"/>
+        <s v="Freddie Mac"/>
+        <s v="Julius Baer"/>
+        <s v="MFR, Inc."/>
+        <s v="Northern Trust"/>
+        <s v="PNC Financial"/>
+        <s v="Point Loma Nazaren Uni…"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Code" numFmtId="0">
+      <sharedItems count="73">
+        <s v="BRA"/>
+        <s v="ACS"/>
+        <s v="AVL"/>
+        <s v="AXA"/>
+        <s v="BOA"/>
+        <s v="BTW"/>
+        <s v="BAR"/>
+        <s v="BBB"/>
+        <s v="BGB"/>
+        <s v="BIE"/>
+        <s v="BM"/>
+        <s v="CIB"/>
+        <s v="CE"/>
+        <s v="CMG"/>
+        <s v="CEA"/>
+        <s v="CB"/>
+        <s v="CAG"/>
+        <s v="CSU"/>
+        <s v="DES"/>
+        <s v="DB"/>
+        <s v="EUL"/>
+        <s v="FNM"/>
+        <s v="FTA"/>
+        <s v="FTN"/>
+        <s v="GSU"/>
+        <s v="HLA"/>
+        <s v="HFE"/>
+        <s v="HUG"/>
+        <s v="GLO"/>
+        <s v="IG"/>
+        <s v="JPM"/>
+        <s v="KSU"/>
+        <s v="KPM"/>
+        <s v="MA"/>
+        <s v="MFN"/>
+        <s v="MOO"/>
+        <s v="BTM"/>
+        <s v="NEA"/>
+        <s v="NAH"/>
+        <s v="NBF"/>
+        <s v="NTE"/>
+        <s v="NS"/>
+        <s v="NRD"/>
+        <s v="OXE"/>
+        <s v="PMA"/>
+        <s v="PRS"/>
+        <s v="PPS"/>
+        <s v="PJC"/>
+        <s v="PRT"/>
+        <s v="RAB"/>
+        <s v="RZB"/>
+        <s v="RJF"/>
+        <s v="RFG"/>
+        <s v="RF"/>
+        <s v="SCA"/>
+        <s v="SMN"/>
+        <s v="SF"/>
+        <s v="SWR"/>
+        <s v="TDS"/>
+        <s v="UMB"/>
+        <s v="UCM"/>
+        <s v="UMD"/>
+        <s v="UTE"/>
+        <s v="USC"/>
+        <s v="VS"/>
+        <s v="WF"/>
+        <s v="CIT"/>
+        <s v="FRM"/>
+        <s v="JBC"/>
+        <s v="MFR"/>
+        <s v="NTR"/>
+        <s v="PNC"/>
+        <s v="PNU"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Ticker" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="74">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="ECGDUS Q117 BRA Index"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="ECGDUS Q117 ACS Index"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="ECGDUS Q117 AVL Index"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="ECGDUS Q117 AXA Index"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="ECGDUS Q117 BOA Index"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="ECGDUS Q117 BTW Index"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="6"/>
+    <s v="ECGDUS Q117 BAR Index"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="7"/>
+    <s v="ECGDUS Q117 BBB Index"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="8"/>
+    <s v="ECGDUS Q117 BGB Index"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="9"/>
+    <s v="ECGDUS Q117 BIE Index"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="10"/>
+    <s v="ECGDUS Q117 BM Index"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="11"/>
+    <s v="ECGDUS Q117 CIB Index"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="12"/>
+    <s v="ECGDUS Q117 CE Index"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="13"/>
+    <s v="ECGDUS Q117 CMG Index"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="14"/>
+    <s v="ECGDUS Q117 CEA Index"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="15"/>
+    <s v="ECGDUS Q117 CB Index"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="16"/>
+    <s v="ECGDUS Q117 CAG Index"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="17"/>
+    <s v="ECGDUS Q117 CSU Index"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <x v="18"/>
+    <s v="ECGDUS Q117 DES Index"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="19"/>
+    <s v="ECGDUS Q117 DB Index"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="20"/>
+    <s v="ECGDUS Q117 EUL Index"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <x v="21"/>
+    <s v="ECGDUS Q117 FNM Index"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="22"/>
+    <s v="ECGDUS Q117 FTA Index"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <x v="23"/>
+    <s v="ECGDUS Q117 FTN Index"/>
+  </r>
+  <r>
+    <x v="24"/>
+    <x v="24"/>
+    <s v="ECGDUS Q117 GSU Index"/>
+  </r>
+  <r>
+    <x v="25"/>
+    <x v="24"/>
+    <s v="ECGDUS Q117 GSU Index"/>
+  </r>
+  <r>
+    <x v="26"/>
+    <x v="25"/>
+    <s v="ECGDUS Q117 HLA Index"/>
+  </r>
+  <r>
+    <x v="27"/>
+    <x v="26"/>
+    <s v="ECGDUS Q117 HFE Index"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <x v="27"/>
+    <s v="ECGDUS Q117 HUG Index"/>
+  </r>
+  <r>
+    <x v="29"/>
+    <x v="28"/>
+    <s v="ECGDUS Q117 GLO Index"/>
+  </r>
+  <r>
+    <x v="30"/>
+    <x v="29"/>
+    <s v="ECGDUS Q117 IG Index"/>
+  </r>
+  <r>
+    <x v="31"/>
+    <x v="30"/>
+    <s v="ECGDUS Q117 JPM Index"/>
+  </r>
+  <r>
+    <x v="32"/>
+    <x v="31"/>
+    <s v="ECGDUS Q117 KSU Index"/>
+  </r>
+  <r>
+    <x v="33"/>
+    <x v="32"/>
+    <s v="ECGDUS Q117 KPM Index"/>
+  </r>
+  <r>
+    <x v="34"/>
+    <x v="33"/>
+    <s v="ECGDUS Q117 MA Index"/>
+  </r>
+  <r>
+    <x v="35"/>
+    <x v="34"/>
+    <s v="ECGDUS Q117 MFN Index"/>
+  </r>
+  <r>
+    <x v="36"/>
+    <x v="35"/>
+    <s v="ECGDUS Q117 MOO Index"/>
+  </r>
+  <r>
+    <x v="37"/>
+    <x v="36"/>
+    <s v="ECGDUS Q117 BTM Index"/>
+  </r>
+  <r>
+    <x v="38"/>
+    <x v="37"/>
+    <s v="ECGDUS Q117 NEA Index"/>
+  </r>
+  <r>
+    <x v="39"/>
+    <x v="38"/>
+    <s v="ECGDUS Q117 NAH Index"/>
+  </r>
+  <r>
+    <x v="40"/>
+    <x v="39"/>
+    <s v="ECGDUS Q117 NBF Index"/>
+  </r>
+  <r>
+    <x v="41"/>
+    <x v="40"/>
+    <s v="ECGDUS Q117 NTE Index"/>
+  </r>
+  <r>
+    <x v="42"/>
+    <x v="41"/>
+    <s v="ECGDUS Q117 NS Index"/>
+  </r>
+  <r>
+    <x v="43"/>
+    <x v="42"/>
+    <s v="ECGDUS Q117 NRD Index"/>
+  </r>
+  <r>
+    <x v="44"/>
+    <x v="43"/>
+    <s v="ECGDUS Q117 OXE Index"/>
+  </r>
+  <r>
+    <x v="45"/>
+    <x v="44"/>
+    <s v="ECGDUS Q117 PMA Index"/>
+  </r>
+  <r>
+    <x v="46"/>
+    <x v="45"/>
+    <s v="ECGDUS Q117 PRS Index"/>
+  </r>
+  <r>
+    <x v="47"/>
+    <x v="46"/>
+    <s v="ECGDUS Q117 PPS Index"/>
+  </r>
+  <r>
+    <x v="48"/>
+    <x v="47"/>
+    <s v="ECGDUS Q117 PJC Index"/>
+  </r>
+  <r>
+    <x v="49"/>
+    <x v="48"/>
+    <s v="ECGDUS Q117 PRT Index"/>
+  </r>
+  <r>
+    <x v="50"/>
+    <x v="49"/>
+    <s v="ECGDUS Q117 RAB Index"/>
+  </r>
+  <r>
+    <x v="51"/>
+    <x v="50"/>
+    <s v="ECGDUS Q117 RZB Index"/>
+  </r>
+  <r>
+    <x v="52"/>
+    <x v="51"/>
+    <s v="ECGDUS Q117 RJF Index"/>
+  </r>
+  <r>
+    <x v="53"/>
+    <x v="52"/>
+    <s v="ECGDUS Q117 RFG Index"/>
+  </r>
+  <r>
+    <x v="54"/>
+    <x v="53"/>
+    <s v="ECGDUS Q117 RF Index"/>
+  </r>
+  <r>
+    <x v="55"/>
+    <x v="54"/>
+    <s v="ECGDUS Q117 SCA Index"/>
+  </r>
+  <r>
+    <x v="56"/>
+    <x v="55"/>
+    <s v="ECGDUS Q117 SMN Index"/>
+  </r>
+  <r>
+    <x v="57"/>
+    <x v="56"/>
+    <s v="ECGDUS Q117 SF Index"/>
+  </r>
+  <r>
+    <x v="58"/>
+    <x v="57"/>
+    <s v="ECGDUS Q117 SWR Index"/>
+  </r>
+  <r>
+    <x v="59"/>
+    <x v="58"/>
+    <s v="ECGDUS Q117 TDS Index"/>
+  </r>
+  <r>
+    <x v="60"/>
+    <x v="59"/>
+    <s v="ECGDUS Q117 UMB Index"/>
+  </r>
+  <r>
+    <x v="61"/>
+    <x v="60"/>
+    <s v="ECGDUS Q117 UCM Index"/>
+  </r>
+  <r>
+    <x v="62"/>
+    <x v="61"/>
+    <s v="ECGDUS Q117 UMD Index"/>
+  </r>
+  <r>
+    <x v="63"/>
+    <x v="62"/>
+    <s v="ECGDUS Q117 UTE Index"/>
+  </r>
+  <r>
+    <x v="64"/>
+    <x v="63"/>
+    <s v="ECGDUS Q117 USC Index"/>
+  </r>
+  <r>
+    <x v="65"/>
+    <x v="64"/>
+    <s v="ECGDUS Q117 VS Index"/>
+  </r>
+  <r>
+    <x v="66"/>
+    <x v="65"/>
+    <s v="ECGDUS Q117 WF Index"/>
+  </r>
+  <r>
+    <x v="67"/>
+    <x v="66"/>
+    <s v="ECGDUS Q117 CIT Index"/>
+  </r>
+  <r>
+    <x v="68"/>
+    <x v="67"/>
+    <s v="ECGDUS Q117 FRM Index"/>
+  </r>
+  <r>
+    <x v="69"/>
+    <x v="68"/>
+    <s v="ECGDUS Q117 JBC Index"/>
+  </r>
+  <r>
+    <x v="70"/>
+    <x v="69"/>
+    <s v="ECGDUS Q117 MFR Index"/>
+  </r>
+  <r>
+    <x v="71"/>
+    <x v="70"/>
+    <s v="ECGDUS Q117 NTR Index"/>
+  </r>
+  <r>
+    <x v="72"/>
+    <x v="71"/>
+    <s v="ECGDUS Q117 PNC Index"/>
+  </r>
+  <r>
+    <x v="73"/>
+    <x v="72"/>
+    <s v="ECGDUS Q117 PNU Index"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A3:B78" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="74">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="67"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="68"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="29"/>
+        <item x="28"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="69"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="70"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="71"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="73">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="36"/>
+        <item x="5"/>
+        <item x="16"/>
+        <item x="15"/>
+        <item x="12"/>
+        <item x="14"/>
+        <item x="11"/>
+        <item x="66"/>
+        <item x="13"/>
+        <item x="17"/>
+        <item x="19"/>
+        <item x="18"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="67"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="28"/>
+        <item x="24"/>
+        <item x="26"/>
+        <item x="25"/>
+        <item x="27"/>
+        <item x="29"/>
+        <item x="68"/>
+        <item x="30"/>
+        <item x="32"/>
+        <item x="31"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="69"/>
+        <item x="35"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="37"/>
+        <item x="42"/>
+        <item x="41"/>
+        <item x="40"/>
+        <item x="70"/>
+        <item x="43"/>
+        <item x="47"/>
+        <item x="44"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="46"/>
+        <item x="45"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="53"/>
+        <item x="52"/>
+        <item x="51"/>
+        <item x="50"/>
+        <item x="54"/>
+        <item x="56"/>
+        <item x="55"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="60"/>
+        <item x="59"/>
+        <item x="61"/>
+        <item x="63"/>
+        <item x="62"/>
+        <item x="64"/>
+        <item x="65"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="75">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="6"/>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="7"/>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="8"/>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="9"/>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="10"/>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="11"/>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="12"/>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="13"/>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="14"/>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="15"/>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="17"/>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="18"/>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="19"/>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="20"/>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="22"/>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="23"/>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="24"/>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="26"/>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="27"/>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="28"/>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="29"/>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="31"/>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="34"/>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="35"/>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="36"/>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="37"/>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="40"/>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="42"/>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="43"/>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="44"/>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="45"/>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="46"/>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="47"/>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="48"/>
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="49"/>
+      <x v="48"/>
+    </i>
+    <i>
+      <x v="50"/>
+      <x v="50"/>
+    </i>
+    <i>
+      <x v="51"/>
+      <x v="54"/>
+    </i>
+    <i>
+      <x v="52"/>
+      <x v="53"/>
+    </i>
+    <i>
+      <x v="53"/>
+      <x v="49"/>
+    </i>
+    <i>
+      <x v="54"/>
+      <x v="51"/>
+    </i>
+    <i>
+      <x v="55"/>
+      <x v="52"/>
+    </i>
+    <i>
+      <x v="56"/>
+      <x v="55"/>
+    </i>
+    <i>
+      <x v="57"/>
+      <x v="56"/>
+    </i>
+    <i>
+      <x v="58"/>
+      <x v="60"/>
+    </i>
+    <i>
+      <x v="59"/>
+      <x v="59"/>
+    </i>
+    <i>
+      <x v="60"/>
+      <x v="58"/>
+    </i>
+    <i>
+      <x v="61"/>
+      <x v="57"/>
+    </i>
+    <i>
+      <x v="62"/>
+      <x v="61"/>
+    </i>
+    <i>
+      <x v="63"/>
+      <x v="63"/>
+    </i>
+    <i>
+      <x v="64"/>
+      <x v="62"/>
+    </i>
+    <i>
+      <x v="65"/>
+      <x v="64"/>
+    </i>
+    <i>
+      <x v="66"/>
+      <x v="65"/>
+    </i>
+    <i>
+      <x v="67"/>
+      <x v="67"/>
+    </i>
+    <i>
+      <x v="68"/>
+      <x v="66"/>
+    </i>
+    <i>
+      <x v="69"/>
+      <x v="68"/>
+    </i>
+    <i>
+      <x v="70"/>
+      <x v="70"/>
+    </i>
+    <i>
+      <x v="71"/>
+      <x v="69"/>
+    </i>
+    <i>
+      <x v="72"/>
+      <x v="71"/>
+    </i>
+    <i>
+      <x v="73"/>
+      <x v="72"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -841,11 +1875,635 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:B78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>135</v>
+      </c>
+      <c r="B28" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>136</v>
+      </c>
+      <c r="B38" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>137</v>
+      </c>
+      <c r="B43" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>74</v>
+      </c>
+      <c r="B49" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>75</v>
+      </c>
+      <c r="B50" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>145</v>
+      </c>
+      <c r="B52" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>91</v>
+      </c>
+      <c r="B55" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>92</v>
+      </c>
+      <c r="B56" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>138</v>
+      </c>
+      <c r="B58" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>139</v>
+      </c>
+      <c r="B59" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>94</v>
+      </c>
+      <c r="B60" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>95</v>
+      </c>
+      <c r="B61" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>96</v>
+      </c>
+      <c r="B62" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>97</v>
+      </c>
+      <c r="B63" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>98</v>
+      </c>
+      <c r="B64" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>99</v>
+      </c>
+      <c r="B65" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>111</v>
+      </c>
+      <c r="B66" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>112</v>
+      </c>
+      <c r="B67" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>113</v>
+      </c>
+      <c r="B68" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>114</v>
+      </c>
+      <c r="B69" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>115</v>
+      </c>
+      <c r="B70" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>116</v>
+      </c>
+      <c r="B71" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>117</v>
+      </c>
+      <c r="B72" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>118</v>
+      </c>
+      <c r="B73" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>119</v>
+      </c>
+      <c r="B74" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>120</v>
+      </c>
+      <c r="B75" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>121</v>
+      </c>
+      <c r="B76" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>133</v>
+      </c>
+      <c r="B77" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1756,18 +3414,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1781,4 +3427,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>